<commit_message>
Update PM17 Tidsregistrering for Tommy.xlsx
</commit_message>
<xml_diff>
--- a/08 Project Management/Tidsregistrering/PM17 Tidsregistrering for Tommy.xlsx
+++ b/08 Project Management/Tidsregistrering/PM17 Tidsregistrering for Tommy.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tommy\Documents\EASJ\Systemudvikling\Projekt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A458F2A-8522-4214-A5B5-8CC3DCE7080D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08BD437C-4BB8-45E5-9B44-722BAC1B91AC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{84363544-26A8-43A0-AC4F-33AAA0FF1AA4}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="60">
   <si>
     <t>Dato</t>
   </si>
@@ -197,6 +197,24 @@
   </si>
   <si>
     <t>Tidsregistrering for Tommy</t>
+  </si>
+  <si>
+    <t>Gør klar og lav brugertest med HØK</t>
+  </si>
+  <si>
+    <t>15 min</t>
+  </si>
+  <si>
+    <t>Lav DOM05 beregn markedsføringsbidrag</t>
+  </si>
+  <si>
+    <t>Kundemøde med HØK</t>
+  </si>
+  <si>
+    <t>45 min</t>
+  </si>
+  <si>
+    <t>Lav UC05 beregn markedsføringsbidrag</t>
   </si>
 </sst>
 </file>
@@ -836,7 +854,7 @@
   <dimension ref="A1:H47"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="66" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1058,7 +1076,7 @@
         <v>49</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C9" s="13">
         <v>43886</v>
@@ -1138,55 +1156,113 @@
       </c>
     </row>
     <row r="12" spans="1:8" ht="19.8" x14ac:dyDescent="0.4">
-      <c r="C12" s="13"/>
-      <c r="D12" s="14"/>
-      <c r="E12" s="14"/>
+      <c r="A12" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" s="13">
+        <v>43887</v>
+      </c>
+      <c r="D12" s="14">
+        <v>0.43055555555555558</v>
+      </c>
+      <c r="E12" s="14">
+        <v>0.49305555555555558</v>
+      </c>
       <c r="F12" s="18"/>
       <c r="G12" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>6.25E-2</v>
       </c>
       <c r="H12" s="1">
         <f>SUM(G$3:G12)</f>
-        <v>0.49305555555555508</v>
+        <v>0.55555555555555514</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="19.8" x14ac:dyDescent="0.4">
-      <c r="C13" s="13"/>
-      <c r="D13" s="14"/>
-      <c r="E13" s="14"/>
-      <c r="F13" s="18"/>
+      <c r="A13" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" s="13">
+        <v>43887</v>
+      </c>
+      <c r="D13" s="14">
+        <v>0.52083333333333337</v>
+      </c>
+      <c r="E13" s="14">
+        <v>0.5625</v>
+      </c>
+      <c r="F13" s="18" t="s">
+        <v>58</v>
+      </c>
       <c r="G13" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4.166666666666663E-2</v>
       </c>
       <c r="H13" s="1">
         <f>SUM(G$3:G13)</f>
-        <v>0.49305555555555508</v>
+        <v>0.59722222222222177</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="19.8" x14ac:dyDescent="0.4">
-      <c r="C14" s="13"/>
-      <c r="F14" s="18"/>
+      <c r="A14" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="B14" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C14" s="13">
+        <v>43887</v>
+      </c>
+      <c r="D14" s="15">
+        <v>0.5625</v>
+      </c>
+      <c r="E14" s="15">
+        <v>0.57638888888888895</v>
+      </c>
+      <c r="F14" s="18" t="s">
+        <v>55</v>
+      </c>
       <c r="G14" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1.3888888888888951E-2</v>
       </c>
       <c r="H14" s="1">
         <f>SUM(G$3:G14)</f>
-        <v>0.49305555555555508</v>
+        <v>0.61111111111111072</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="19.8" x14ac:dyDescent="0.4">
-      <c r="C15" s="13"/>
-      <c r="F15" s="18"/>
+      <c r="A15" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="B15" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C15" s="13">
+        <v>43887</v>
+      </c>
+      <c r="D15" s="15">
+        <v>0.57638888888888895</v>
+      </c>
+      <c r="E15" s="15">
+        <v>0.59027777777777779</v>
+      </c>
+      <c r="F15" s="18" t="s">
+        <v>55</v>
+      </c>
       <c r="G15" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1.388888888888884E-2</v>
       </c>
       <c r="H15" s="1">
         <f>SUM(G$3:G15)</f>
-        <v>0.49305555555555508</v>
+        <v>0.62499999999999956</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="19.8" x14ac:dyDescent="0.4">
@@ -1198,7 +1274,7 @@
       </c>
       <c r="H16" s="1">
         <f>SUM(G$3:G16)</f>
-        <v>0.49305555555555508</v>
+        <v>0.62499999999999956</v>
       </c>
     </row>
     <row r="17" spans="3:8" ht="19.8" x14ac:dyDescent="0.4">
@@ -1210,7 +1286,7 @@
       </c>
       <c r="H17" s="1">
         <f>SUM(G$3:G17)</f>
-        <v>0.49305555555555508</v>
+        <v>0.62499999999999956</v>
       </c>
     </row>
     <row r="18" spans="3:8" ht="19.8" x14ac:dyDescent="0.4">
@@ -1222,7 +1298,7 @@
       </c>
       <c r="H18" s="1">
         <f>SUM(G$3:G18)</f>
-        <v>0.49305555555555508</v>
+        <v>0.62499999999999956</v>
       </c>
     </row>
     <row r="19" spans="3:8" ht="19.8" x14ac:dyDescent="0.4">
@@ -1234,7 +1310,7 @@
       </c>
       <c r="H19" s="1">
         <f>SUM(G$3:G19)</f>
-        <v>0.49305555555555508</v>
+        <v>0.62499999999999956</v>
       </c>
     </row>
     <row r="20" spans="3:8" ht="19.8" x14ac:dyDescent="0.4">
@@ -1246,7 +1322,7 @@
       </c>
       <c r="H20" s="1">
         <f>SUM(G$3:G20)</f>
-        <v>0.49305555555555508</v>
+        <v>0.62499999999999956</v>
       </c>
     </row>
     <row r="21" spans="3:8" ht="19.8" x14ac:dyDescent="0.4">
@@ -1258,7 +1334,7 @@
       </c>
       <c r="H21" s="1">
         <f>SUM(G$3:G21)</f>
-        <v>0.49305555555555508</v>
+        <v>0.62499999999999956</v>
       </c>
     </row>
     <row r="22" spans="3:8" ht="19.8" x14ac:dyDescent="0.4">
@@ -1270,7 +1346,7 @@
       </c>
       <c r="H22" s="1">
         <f>SUM(G$3:G22)</f>
-        <v>0.49305555555555508</v>
+        <v>0.62499999999999956</v>
       </c>
     </row>
     <row r="23" spans="3:8" ht="19.8" x14ac:dyDescent="0.4">
@@ -1282,7 +1358,7 @@
       </c>
       <c r="H23" s="1">
         <f>SUM(G$3:G23)</f>
-        <v>0.49305555555555508</v>
+        <v>0.62499999999999956</v>
       </c>
     </row>
     <row r="24" spans="3:8" ht="19.8" x14ac:dyDescent="0.4">
@@ -1294,7 +1370,7 @@
       </c>
       <c r="H24" s="1">
         <f>SUM(G$3:G24)</f>
-        <v>0.49305555555555508</v>
+        <v>0.62499999999999956</v>
       </c>
     </row>
     <row r="25" spans="3:8" ht="19.8" x14ac:dyDescent="0.4">
@@ -1305,7 +1381,7 @@
       </c>
       <c r="H25" s="1">
         <f>SUM(G$3:G25)</f>
-        <v>0.49305555555555508</v>
+        <v>0.62499999999999956</v>
       </c>
     </row>
     <row r="26" spans="3:8" ht="19.8" x14ac:dyDescent="0.4">
@@ -1316,7 +1392,7 @@
       </c>
       <c r="H26" s="1">
         <f>SUM(G$3:G26)</f>
-        <v>0.49305555555555508</v>
+        <v>0.62499999999999956</v>
       </c>
     </row>
     <row r="27" spans="3:8" ht="19.8" x14ac:dyDescent="0.4">
@@ -1327,7 +1403,7 @@
       </c>
       <c r="H27" s="1">
         <f>SUM(G$3:G27)</f>
-        <v>0.49305555555555508</v>
+        <v>0.62499999999999956</v>
       </c>
     </row>
     <row r="28" spans="3:8" ht="19.8" x14ac:dyDescent="0.4">
@@ -1338,7 +1414,7 @@
       </c>
       <c r="H28" s="1">
         <f>SUM(G$3:G28)</f>
-        <v>0.49305555555555508</v>
+        <v>0.62499999999999956</v>
       </c>
     </row>
     <row r="29" spans="3:8" ht="19.8" x14ac:dyDescent="0.4">
@@ -1349,7 +1425,7 @@
       </c>
       <c r="H29" s="1">
         <f>SUM(G$3:G29)</f>
-        <v>0.49305555555555508</v>
+        <v>0.62499999999999956</v>
       </c>
     </row>
     <row r="30" spans="3:8" ht="19.8" x14ac:dyDescent="0.4">
@@ -1360,7 +1436,7 @@
       </c>
       <c r="H30" s="1">
         <f>SUM(G$3:G30)</f>
-        <v>0.49305555555555508</v>
+        <v>0.62499999999999956</v>
       </c>
     </row>
     <row r="31" spans="3:8" ht="19.8" x14ac:dyDescent="0.4">
@@ -1371,7 +1447,7 @@
       </c>
       <c r="H31" s="1">
         <f>SUM(G$3:G31)</f>
-        <v>0.49305555555555508</v>
+        <v>0.62499999999999956</v>
       </c>
     </row>
     <row r="32" spans="3:8" ht="19.8" x14ac:dyDescent="0.4">
@@ -1382,7 +1458,7 @@
       </c>
       <c r="H32" s="1">
         <f>SUM(G$3:G32)</f>
-        <v>0.49305555555555508</v>
+        <v>0.62499999999999956</v>
       </c>
     </row>
     <row r="33" spans="3:3" x14ac:dyDescent="0.3">

</xml_diff>